<commit_message>
Complete code for an email automation
</commit_message>
<xml_diff>
--- a/TestData/MailTestData.xlsx
+++ b/TestData/MailTestData.xlsx
@@ -28,13 +28,13 @@
     <t>Archive an email</t>
   </si>
   <si>
-    <t>ajithkumar.j@optisolbusiness.com</t>
+    <t>arun.chandra@anywhere.co</t>
   </si>
   <si>
     <t>Automation</t>
   </si>
   <si>
-    <t>Script</t>
+    <t>Hi this is an automation mail</t>
   </si>
 </sst>
 </file>
@@ -43,9 +43,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -56,47 +56,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -141,6 +133,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -150,21 +180,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -172,7 +187,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -180,21 +195,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,139 +221,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -365,37 +395,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,17 +420,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,6 +487,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -542,141 +542,144 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1000,14 +1003,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="31.4545454545455" customWidth="1"/>
     <col min="2" max="2" width="20.5454545454545" customWidth="1"/>
-    <col min="3" max="3" width="19.7272727272727" customWidth="1"/>
+    <col min="3" max="3" width="29.9090909090909" customWidth="1"/>
     <col min="4" max="4" width="31.5454545454545" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1032,7 +1035,7 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1040,6 +1043,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="arun.chandra@anywhere.co" tooltip="mailto:arun.chandra@anywhere.co"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>

</xml_diff>